<commit_message>
[ADD] add kleos space to all plots
</commit_message>
<xml_diff>
--- a/financial_data/kleos.xlsx
+++ b/financial_data/kleos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F626EE5-B8EF-45F9-A080-A8A1101D6B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F97E4B-D814-4606-9FC7-714CEECB43CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,8 +188,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="169" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -253,13 +253,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430E7A42-4932-4281-BA35-B8BB0DF46295}">
   <dimension ref="A1:AX18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1373,7 +1373,9 @@
       <c r="R6" s="6">
         <v>0</v>
       </c>
-      <c r="S6" s="6"/>
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
       <c r="T6" s="6">
         <v>2192066</v>
       </c>

</xml_diff>